<commit_message>
Automatische test-sync: 2025-07-29 21:28:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-29.xlsx
+++ b/logs/mail_log_2025-07-29.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -730,8 +730,55 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-07-29 21:28:46</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2">
+  <conditionalFormatting sqref="D2:D3">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -751,7 +798,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2">
+  <conditionalFormatting sqref="G2:G3">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -759,17 +806,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
+  <conditionalFormatting sqref="H2:H3">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
+  <conditionalFormatting sqref="I2:I3">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2">
+  <conditionalFormatting sqref="J2:J3">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -811,7 +858,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-29 21:31:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-29.xlsx
+++ b/logs/mail_log_2025-07-29.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2</f>
+              <f>'Dashboard'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2</f>
+              <f>'Dashboard'!$B$2:$B$3</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -777,8 +777,55 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Wil je dit oppakken?</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Testmail #2: Wil je dit oppakken?</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-07-29 21:30:57</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D3">
+  <conditionalFormatting sqref="D2:D4">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -798,7 +845,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3">
+  <conditionalFormatting sqref="G2:G4">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -806,17 +853,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H3">
+  <conditionalFormatting sqref="H2:H4">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I3">
+  <conditionalFormatting sqref="I2:I4">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J3">
+  <conditionalFormatting sqref="J2:J4">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -831,7 +878,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -861,6 +908,16 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-29 21:33:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-29.xlsx
+++ b/logs/mail_log_2025-07-29.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -824,8 +824,55 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Kun jij dit afhandelen?</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Testmail #3: Kun jij dit afhandelen?</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-07-29 21:33:10</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D4">
+  <conditionalFormatting sqref="D2:D5">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -845,7 +892,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G4">
+  <conditionalFormatting sqref="G2:G5">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -853,17 +900,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H4">
+  <conditionalFormatting sqref="H2:H5">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I4">
+  <conditionalFormatting sqref="I2:I5">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J4">
+  <conditionalFormatting sqref="J2:J5">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -905,7 +952,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-29 21:42:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-29.xlsx
+++ b/logs/mail_log_2025-07-29.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1038,8 +1038,55 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Is dit artikel nog op voorraad?</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Testmail #7: Is dit artikel nog op voorraad?</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-07-29 21:41:54</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D8">
+  <conditionalFormatting sqref="D2:D9">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1059,7 +1106,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G8">
+  <conditionalFormatting sqref="G2:G9">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1067,17 +1114,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H8">
+  <conditionalFormatting sqref="H2:H9">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I8">
+  <conditionalFormatting sqref="I2:I9">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J8">
+  <conditionalFormatting sqref="J2:J9">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1135,17 +1182,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Bestelling / Levering</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Bestelling / Levering</t>
         </is>
       </c>
       <c r="B5" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-29 21:46:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-29.xlsx
+++ b/logs/mail_log_2025-07-29.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1140,8 +1140,55 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Hoi, hebben jullie al iets gehoord?</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Testmail #9: Hoi, hebben jullie al iets gehoord?</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-07-29 21:46:16</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D10">
+  <conditionalFormatting sqref="D2:D11">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1161,7 +1208,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G10">
+  <conditionalFormatting sqref="G2:G11">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1169,17 +1216,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H10">
+  <conditionalFormatting sqref="H2:H11">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I10">
+  <conditionalFormatting sqref="I2:I11">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J10">
+  <conditionalFormatting sqref="J2:J11">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1221,7 +1268,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-29 21:49:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-29.xlsx
+++ b/logs/mail_log_2025-07-29.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1187,8 +1187,55 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Is er al nieuws?</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Testmail #10: Is er al nieuws?</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-07-29 21:48:54</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D11">
+  <conditionalFormatting sqref="D2:D12">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1208,7 +1255,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G11">
+  <conditionalFormatting sqref="G2:G12">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1216,17 +1263,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H11">
+  <conditionalFormatting sqref="H2:H12">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I11">
+  <conditionalFormatting sqref="I2:I12">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J11">
+  <conditionalFormatting sqref="J2:J12">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1274,7 +1321,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Intern verzoek / Actie voor medewerker</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1284,11 +1331,11 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Intern verzoek / Actie voor medewerker</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-29 22:00:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-29.xlsx
+++ b/logs/mail_log_2025-07-29.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1459,8 +1459,55 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Leg dit even neer bij Koen.</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Testmail #15: Leg dit even neer bij Koen.</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025-07-29 21:59:52</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D16">
+  <conditionalFormatting sqref="D2:D17">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1480,7 +1527,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G16">
+  <conditionalFormatting sqref="G2:G17">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1488,17 +1535,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H16">
+  <conditionalFormatting sqref="H2:H17">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I16">
+  <conditionalFormatting sqref="I2:I17">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J16">
+  <conditionalFormatting sqref="J2:J17">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1560,7 +1607,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-29 22:02:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-29.xlsx
+++ b/logs/mail_log_2025-07-29.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1506,8 +1506,55 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Wil je dit even doorsturen?</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Testmail #16: Wil je dit even doorsturen?</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-07-29 22:02:06</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D17">
+  <conditionalFormatting sqref="D2:D18">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1527,7 +1574,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G17">
+  <conditionalFormatting sqref="G2:G18">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1535,17 +1582,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H17">
+  <conditionalFormatting sqref="H2:H18">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I17">
+  <conditionalFormatting sqref="I2:I18">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J17">
+  <conditionalFormatting sqref="J2:J18">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1583,7 +1630,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -1593,11 +1640,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-29 22:09:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-29.xlsx
+++ b/logs/mail_log_2025-07-29.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1663,8 +1663,55 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Bel jij klant Jansen even?</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Testmail #19: Bel jij klant Jansen even?</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2025-07-29 22:08:55</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D20">
+  <conditionalFormatting sqref="D2:D21">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1684,7 +1731,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G20">
+  <conditionalFormatting sqref="G2:G21">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1692,17 +1739,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H20">
+  <conditionalFormatting sqref="H2:H21">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I20">
+  <conditionalFormatting sqref="I2:I21">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J20">
+  <conditionalFormatting sqref="J2:J21">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1750,7 +1797,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Intern verzoek / Actie voor medewerker</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1760,11 +1807,11 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Intern verzoek / Actie voor medewerker</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-29 22:11:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-29.xlsx
+++ b/logs/mail_log_2025-07-29.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$7</f>
+              <f>'Dashboard'!$A$2:$A$8</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$7</f>
+              <f>'Dashboard'!$B$2:$B$8</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1710,8 +1710,55 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Ik ben niet tevreden over hoe dit is gegaan.</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Testmail #20: Ik ben niet tevreden over hoe dit is gegaan.</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Klacht / Probleem</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2025-07-29 22:11:06</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D21">
+  <conditionalFormatting sqref="D2:D22">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1731,7 +1778,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G21">
+  <conditionalFormatting sqref="G2:G22">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1739,17 +1786,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H21">
+  <conditionalFormatting sqref="H2:H22">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I21">
+  <conditionalFormatting sqref="I2:I22">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J21">
+  <conditionalFormatting sqref="J2:J22">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1764,7 +1811,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1844,6 +1891,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Klacht / Probleem</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>